<commit_message>
Adiciona exportação com xlsxwriter e remove indicador sem localização
</commit_message>
<xml_diff>
--- a/Feedback_Localizacao.xlsx
+++ b/Feedback_Localizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.lucio\Desktop\localizacao-produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BCB6B7-71BE-4228-980B-AD0B40C1B543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575F0D6D-E338-49AC-84AB-8639146FD1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{465510BC-D290-4320-95D4-F9D384AF176B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="183">
   <si>
     <t>SEÇÃO</t>
   </si>
@@ -567,6 +567,24 @@
   </si>
   <si>
     <t>RACAO WHISKAS FRANGO KG</t>
+  </si>
+  <si>
+    <t>LIMPEZA</t>
+  </si>
+  <si>
+    <t>MERCEARIA DOCE</t>
+  </si>
+  <si>
+    <t>MERCEARIA SALGADA</t>
+  </si>
+  <si>
+    <t>PERFUMARIA</t>
+  </si>
+  <si>
+    <t>PERFUMARIA INFANTIL</t>
+  </si>
+  <si>
+    <t>PETSHOP</t>
   </si>
 </sst>
 </file>
@@ -991,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F920F512-DBD9-4CCD-97A3-ACB65F137278}">
   <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,6 +1085,9 @@
       <c r="G2" s="3">
         <v>55</v>
       </c>
+      <c r="H2" t="s">
+        <v>177</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -1093,6 +1114,9 @@
       <c r="G3" s="3">
         <v>15</v>
       </c>
+      <c r="H3" t="s">
+        <v>177</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3"/>
       <c r="L3"/>
@@ -1119,6 +1143,9 @@
       <c r="G4" s="3">
         <v>32</v>
       </c>
+      <c r="H4" t="s">
+        <v>177</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -1145,6 +1172,9 @@
       <c r="G5" s="3">
         <v>16</v>
       </c>
+      <c r="H5" t="s">
+        <v>177</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -1171,6 +1201,9 @@
       <c r="G6" s="3">
         <v>43</v>
       </c>
+      <c r="H6" t="s">
+        <v>177</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -1197,6 +1230,9 @@
       <c r="G7" s="3">
         <v>14</v>
       </c>
+      <c r="H7" t="s">
+        <v>177</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -1223,6 +1259,9 @@
       <c r="G8" s="3">
         <v>67</v>
       </c>
+      <c r="H8" t="s">
+        <v>177</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -1249,6 +1288,9 @@
       <c r="G9" s="3">
         <v>15</v>
       </c>
+      <c r="H9" t="s">
+        <v>177</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -1275,6 +1317,9 @@
       <c r="G10" s="3">
         <v>25</v>
       </c>
+      <c r="H10" t="s">
+        <v>177</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -1301,6 +1346,9 @@
       <c r="G11" s="3">
         <v>22</v>
       </c>
+      <c r="H11" t="s">
+        <v>177</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11"/>
       <c r="L11"/>
@@ -1327,6 +1375,9 @@
       <c r="G12" s="3">
         <v>17</v>
       </c>
+      <c r="H12" t="s">
+        <v>177</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -1353,6 +1404,9 @@
       <c r="G13" s="3">
         <v>33</v>
       </c>
+      <c r="H13" t="s">
+        <v>177</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13"/>
       <c r="L13"/>
@@ -1379,6 +1433,9 @@
       <c r="G14" s="3">
         <v>154</v>
       </c>
+      <c r="H14" t="s">
+        <v>177</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14"/>
       <c r="L14"/>
@@ -1405,6 +1462,9 @@
       <c r="G15" s="3">
         <v>18</v>
       </c>
+      <c r="H15" t="s">
+        <v>177</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15"/>
       <c r="L15"/>
@@ -1431,6 +1491,9 @@
       <c r="G16" s="3">
         <v>22</v>
       </c>
+      <c r="H16" t="s">
+        <v>177</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16"/>
       <c r="L16"/>
@@ -1457,6 +1520,9 @@
       <c r="G17" s="3">
         <v>83</v>
       </c>
+      <c r="H17" t="s">
+        <v>177</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17"/>
       <c r="L17"/>
@@ -1483,6 +1549,9 @@
       <c r="G18" s="3">
         <v>16</v>
       </c>
+      <c r="H18" t="s">
+        <v>177</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18"/>
       <c r="L18"/>
@@ -1509,6 +1578,9 @@
       <c r="G19" s="3">
         <v>16</v>
       </c>
+      <c r="H19" t="s">
+        <v>177</v>
+      </c>
       <c r="J19" s="5"/>
       <c r="K19"/>
       <c r="L19"/>
@@ -1535,6 +1607,9 @@
       <c r="G20" s="3">
         <v>88</v>
       </c>
+      <c r="H20" t="s">
+        <v>177</v>
+      </c>
       <c r="J20" s="5"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -1561,6 +1636,9 @@
       <c r="G21" s="3">
         <v>29</v>
       </c>
+      <c r="H21" t="s">
+        <v>177</v>
+      </c>
       <c r="J21" s="5"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -1587,6 +1665,9 @@
       <c r="G22" s="3">
         <v>36</v>
       </c>
+      <c r="H22" t="s">
+        <v>177</v>
+      </c>
       <c r="J22" s="5"/>
       <c r="K22"/>
       <c r="L22"/>
@@ -1613,6 +1694,9 @@
       <c r="G23" s="3">
         <v>15</v>
       </c>
+      <c r="H23" t="s">
+        <v>177</v>
+      </c>
       <c r="J23" s="5"/>
       <c r="K23"/>
       <c r="L23"/>
@@ -1639,6 +1723,9 @@
       <c r="G24" s="3">
         <v>43</v>
       </c>
+      <c r="H24" t="s">
+        <v>177</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24"/>
       <c r="L24"/>
@@ -1665,6 +1752,9 @@
       <c r="G25" s="3">
         <v>77</v>
       </c>
+      <c r="H25" t="s">
+        <v>177</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25"/>
       <c r="L25"/>
@@ -1691,6 +1781,9 @@
       <c r="G26" s="3">
         <v>24</v>
       </c>
+      <c r="H26" t="s">
+        <v>177</v>
+      </c>
       <c r="J26" s="5"/>
       <c r="K26"/>
       <c r="L26"/>
@@ -1717,6 +1810,9 @@
       <c r="G27" s="3">
         <v>20</v>
       </c>
+      <c r="H27" t="s">
+        <v>177</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27"/>
       <c r="L27"/>
@@ -1743,6 +1839,9 @@
       <c r="G28" s="3">
         <v>22</v>
       </c>
+      <c r="H28" t="s">
+        <v>178</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28"/>
       <c r="L28"/>
@@ -1769,6 +1868,9 @@
       <c r="G29" s="3">
         <v>25</v>
       </c>
+      <c r="H29" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1792,6 +1894,9 @@
       <c r="G30" s="3">
         <v>17</v>
       </c>
+      <c r="H30" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1815,6 +1920,9 @@
       <c r="G31" s="3">
         <v>23</v>
       </c>
+      <c r="H31" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1838,8 +1946,11 @@
       <c r="G32" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1861,8 +1972,11 @@
       <c r="G33" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1884,8 +1998,11 @@
       <c r="G34" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1907,8 +2024,11 @@
       <c r="G35" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1930,8 +2050,11 @@
       <c r="G36" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1953,8 +2076,11 @@
       <c r="G37" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1976,8 +2102,11 @@
       <c r="G38" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -1999,8 +2128,11 @@
       <c r="G39" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2022,8 +2154,11 @@
       <c r="G40" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2045,8 +2180,11 @@
       <c r="G41" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2068,8 +2206,11 @@
       <c r="G42" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2091,8 +2232,11 @@
       <c r="G43" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2114,8 +2258,11 @@
       <c r="G44" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2137,8 +2284,11 @@
       <c r="G45" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -2160,8 +2310,11 @@
       <c r="G46" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -2183,8 +2336,11 @@
       <c r="G47" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -2206,8 +2362,11 @@
       <c r="G48" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -2229,8 +2388,11 @@
       <c r="G49" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2252,8 +2414,11 @@
       <c r="G50" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2275,8 +2440,11 @@
       <c r="G51" s="1">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -2298,8 +2466,11 @@
       <c r="G52" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -2321,8 +2492,11 @@
       <c r="G53" s="1">
         <v>133</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -2344,8 +2518,11 @@
       <c r="G54" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -2367,8 +2544,11 @@
       <c r="G55" s="1">
         <v>163</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -2390,8 +2570,11 @@
       <c r="G56" s="1">
         <v>165</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -2413,8 +2596,11 @@
       <c r="G57" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -2436,8 +2622,11 @@
       <c r="G58" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>22</v>
       </c>
@@ -2459,8 +2648,11 @@
       <c r="G59" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -2482,8 +2674,11 @@
       <c r="G60" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -2505,8 +2700,11 @@
       <c r="G61" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -2528,8 +2726,11 @@
       <c r="G62" s="1">
         <v>118</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2551,8 +2752,11 @@
       <c r="G63" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -2574,8 +2778,11 @@
       <c r="G64" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -2597,8 +2804,11 @@
       <c r="G65" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -2620,8 +2830,11 @@
       <c r="G66" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -2643,8 +2856,11 @@
       <c r="G67" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -2666,8 +2882,11 @@
       <c r="G68" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -2689,8 +2908,11 @@
       <c r="G69" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -2712,8 +2934,11 @@
       <c r="G70" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -2735,8 +2960,11 @@
       <c r="G71" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -2758,8 +2986,11 @@
       <c r="G72" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -2781,8 +3012,11 @@
       <c r="G73" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>22</v>
       </c>
@@ -2804,8 +3038,11 @@
       <c r="G74" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>22</v>
       </c>
@@ -2827,8 +3064,11 @@
       <c r="G75" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>22</v>
       </c>
@@ -2850,8 +3090,11 @@
       <c r="G76" s="1">
         <v>88</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>22</v>
       </c>
@@ -2873,8 +3116,11 @@
       <c r="G77" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -2896,8 +3142,11 @@
       <c r="G78" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -2919,8 +3168,11 @@
       <c r="G79" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -2942,8 +3194,11 @@
       <c r="G80" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -2965,8 +3220,11 @@
       <c r="G81" s="1">
         <v>171</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -2988,8 +3246,11 @@
       <c r="G82" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H82" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -3011,8 +3272,11 @@
       <c r="G83" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H83" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>22</v>
       </c>
@@ -3034,8 +3298,11 @@
       <c r="G84" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H84" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -3057,8 +3324,11 @@
       <c r="G85" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H85" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -3080,8 +3350,11 @@
       <c r="G86" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -3103,8 +3376,11 @@
       <c r="G87" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H87" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -3126,8 +3402,11 @@
       <c r="G88" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H88" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -3149,8 +3428,11 @@
       <c r="G89" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -3172,8 +3454,11 @@
       <c r="G90" s="1">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -3195,8 +3480,11 @@
       <c r="G91" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>22</v>
       </c>
@@ -3218,8 +3506,11 @@
       <c r="G92" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H92" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -3241,8 +3532,11 @@
       <c r="G93" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>22</v>
       </c>
@@ -3264,8 +3558,11 @@
       <c r="G94" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H94" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>22</v>
       </c>
@@ -3287,8 +3584,11 @@
       <c r="G95" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H95" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>22</v>
       </c>
@@ -3310,8 +3610,11 @@
       <c r="G96" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>22</v>
       </c>
@@ -3333,8 +3636,11 @@
       <c r="G97" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -3356,8 +3662,11 @@
       <c r="G98" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>22</v>
       </c>
@@ -3379,8 +3688,11 @@
       <c r="G99" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -3402,8 +3714,11 @@
       <c r="G100" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -3425,8 +3740,11 @@
       <c r="G101" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>22</v>
       </c>
@@ -3448,8 +3766,11 @@
       <c r="G102" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -3471,8 +3792,11 @@
       <c r="G103" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -3494,8 +3818,11 @@
       <c r="G104" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>22</v>
       </c>
@@ -3517,8 +3844,11 @@
       <c r="G105" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>22</v>
       </c>
@@ -3540,8 +3870,11 @@
       <c r="G106" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>22</v>
       </c>
@@ -3563,8 +3896,11 @@
       <c r="G107" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>22</v>
       </c>
@@ -3586,8 +3922,11 @@
       <c r="G108" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>22</v>
       </c>
@@ -3609,8 +3948,11 @@
       <c r="G109" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>22</v>
       </c>
@@ -3632,8 +3974,11 @@
       <c r="G110" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>22</v>
       </c>
@@ -3655,8 +4000,11 @@
       <c r="G111" s="1">
         <v>147</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>22</v>
       </c>
@@ -3678,8 +4026,11 @@
       <c r="G112" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H112" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>22</v>
       </c>
@@ -3701,8 +4052,11 @@
       <c r="G113" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H113" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -3724,8 +4078,11 @@
       <c r="G114" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H114" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>22</v>
       </c>
@@ -3747,8 +4104,11 @@
       <c r="G115" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H115" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -3770,8 +4130,11 @@
       <c r="G116" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H116" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -3793,8 +4156,11 @@
       <c r="G117" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H117" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>22</v>
       </c>
@@ -3816,8 +4182,11 @@
       <c r="G118" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H118" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>22</v>
       </c>
@@ -3839,8 +4208,11 @@
       <c r="G119" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H119" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>22</v>
       </c>
@@ -3862,8 +4234,11 @@
       <c r="G120" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H120" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>22</v>
       </c>
@@ -3885,8 +4260,11 @@
       <c r="G121" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H121" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>22</v>
       </c>
@@ -3908,8 +4286,11 @@
       <c r="G122" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H122" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>22</v>
       </c>
@@ -3931,8 +4312,11 @@
       <c r="G123" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H123" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>22</v>
       </c>
@@ -3954,8 +4338,11 @@
       <c r="G124" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H124" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>22</v>
       </c>
@@ -3977,8 +4364,11 @@
       <c r="G125" s="1">
         <v>101</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H125" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>22</v>
       </c>
@@ -4000,8 +4390,11 @@
       <c r="G126" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H126" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>22</v>
       </c>
@@ -4023,8 +4416,11 @@
       <c r="G127" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H127" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>22</v>
       </c>
@@ -4046,8 +4442,11 @@
       <c r="G128" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H128" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>22</v>
       </c>
@@ -4069,8 +4468,11 @@
       <c r="G129" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H129" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -4092,8 +4494,11 @@
       <c r="G130" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H130" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -4115,8 +4520,11 @@
       <c r="G131" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H131" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>22</v>
       </c>
@@ -4138,8 +4546,11 @@
       <c r="G132" s="1">
         <v>97</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H132" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>22</v>
       </c>
@@ -4161,8 +4572,11 @@
       <c r="G133" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H133" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>22</v>
       </c>
@@ -4184,8 +4598,11 @@
       <c r="G134" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>22</v>
       </c>
@@ -4207,8 +4624,11 @@
       <c r="G135" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H135" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>22</v>
       </c>
@@ -4230,8 +4650,11 @@
       <c r="G136" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H136" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>22</v>
       </c>
@@ -4253,8 +4676,11 @@
       <c r="G137" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H137" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>22</v>
       </c>
@@ -4276,8 +4702,11 @@
       <c r="G138" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H138" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>22</v>
       </c>
@@ -4299,8 +4728,11 @@
       <c r="G139" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H139" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>22</v>
       </c>
@@ -4322,8 +4754,11 @@
       <c r="G140" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H140" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>22</v>
       </c>
@@ -4345,8 +4780,11 @@
       <c r="G141" s="1">
         <v>236</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H141" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>22</v>
       </c>
@@ -4368,8 +4806,11 @@
       <c r="G142" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H142" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>22</v>
       </c>
@@ -4391,8 +4832,11 @@
       <c r="G143" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H143" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>22</v>
       </c>
@@ -4414,8 +4858,11 @@
       <c r="G144" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H144" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>22</v>
       </c>
@@ -4437,8 +4884,11 @@
       <c r="G145" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H145" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>22</v>
       </c>
@@ -4460,8 +4910,11 @@
       <c r="G146" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H146" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>22</v>
       </c>
@@ -4483,8 +4936,11 @@
       <c r="G147" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H147" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>22</v>
       </c>
@@ -4506,8 +4962,11 @@
       <c r="G148" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H148" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>22</v>
       </c>
@@ -4529,8 +4988,11 @@
       <c r="G149" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H149" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>22</v>
       </c>
@@ -4552,8 +5014,11 @@
       <c r="G150" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H150" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>22</v>
       </c>
@@ -4575,8 +5040,11 @@
       <c r="G151" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H151" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>22</v>
       </c>
@@ -4598,8 +5066,11 @@
       <c r="G152" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H152" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>22</v>
       </c>
@@ -4621,8 +5092,11 @@
       <c r="G153" s="1">
         <v>85</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H153" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>22</v>
       </c>
@@ -4644,8 +5118,11 @@
       <c r="G154" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H154" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>22</v>
       </c>
@@ -4667,8 +5144,11 @@
       <c r="G155" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H155" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>22</v>
       </c>
@@ -4690,8 +5170,11 @@
       <c r="G156" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H156" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>22</v>
       </c>
@@ -4713,8 +5196,11 @@
       <c r="G157" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H157" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>22</v>
       </c>
@@ -4736,8 +5222,11 @@
       <c r="G158" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H158" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>22</v>
       </c>
@@ -4759,8 +5248,11 @@
       <c r="G159" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H159" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>22</v>
       </c>
@@ -4782,8 +5274,11 @@
       <c r="G160" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H160" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>22</v>
       </c>
@@ -4805,8 +5300,11 @@
       <c r="G161" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H161" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>22</v>
       </c>
@@ -4828,8 +5326,11 @@
       <c r="G162" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H162" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>22</v>
       </c>
@@ -4851,8 +5352,11 @@
       <c r="G163" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H163" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>22</v>
       </c>
@@ -4874,8 +5378,11 @@
       <c r="G164" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H164" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>22</v>
       </c>
@@ -4897,8 +5404,11 @@
       <c r="G165" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H165" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>22</v>
       </c>
@@ -4920,8 +5430,11 @@
       <c r="G166" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H166" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>22</v>
       </c>
@@ -4942,6 +5455,9 @@
       </c>
       <c r="G167" s="1">
         <v>17</v>
+      </c>
+      <c r="H167" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes no autosave e layout do painel admin
</commit_message>
<xml_diff>
--- a/Feedback_Localizacao.xlsx
+++ b/Feedback_Localizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.lucio\Desktop\localizacao-produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F362F17-1399-4265-A215-83576A536AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B6B8A3-0D54-4198-9D13-04763D184832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{465510BC-D290-4320-95D4-F9D384AF176B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="248">
   <si>
     <t>SEÇÃO</t>
   </si>
@@ -123,186 +123,6 @@
   </si>
   <si>
     <t>PRODUTOS SEM VENDA PAN 29/05</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/06</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/07</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/08</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/09</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/10</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/11</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/12</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/13</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/14</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/15</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/16</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/17</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/18</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/19</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/20</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/21</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/22</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/23</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/24</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/25</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/26</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/27</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/28</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/29</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/30</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/31</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/32</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/33</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/34</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/35</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/36</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/37</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/38</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/39</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/40</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/41</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/42</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/43</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/44</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/45</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/46</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/47</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/48</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/49</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/50</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/51</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/52</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/53</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/54</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/55</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/56</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/57</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/58</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/59</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/60</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/61</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/62</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/63</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/64</t>
-  </si>
-  <si>
-    <t>PRODUTOS SEM VENDA PAN 29/65</t>
   </si>
   <si>
     <t>BROCOLIS FLORETE DAUCY CONG.300G</t>
@@ -1384,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F920F512-DBD9-4CCD-97A3-ACB65F137278}">
   <dimension ref="A1:L227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,7 +1266,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>37805</v>
@@ -1461,7 +1281,7 @@
         <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2"/>
@@ -1475,7 +1295,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>37802</v>
@@ -1490,7 +1310,7 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3"/>
@@ -1504,7 +1324,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>37797</v>
@@ -1519,7 +1339,7 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4"/>
@@ -1533,7 +1353,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>37864</v>
@@ -1548,7 +1368,7 @@
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5"/>
@@ -1562,7 +1382,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1356828</v>
@@ -1577,7 +1397,7 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6"/>
@@ -1591,7 +1411,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>37807</v>
@@ -1606,7 +1426,7 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7"/>
@@ -1620,7 +1440,7 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>33677</v>
@@ -1635,7 +1455,7 @@
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8"/>
@@ -1649,7 +1469,7 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>1356917</v>
@@ -1664,7 +1484,7 @@
         <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9"/>
@@ -1678,7 +1498,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>36541</v>
@@ -1693,7 +1513,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10"/>
@@ -1707,7 +1527,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>722480</v>
@@ -1722,7 +1542,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11"/>
@@ -1736,7 +1556,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>31436</v>
@@ -1751,7 +1571,7 @@
         <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12"/>
@@ -1765,7 +1585,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>1110985</v>
@@ -1780,7 +1600,7 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13"/>
@@ -1794,7 +1614,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>18099</v>
@@ -1809,7 +1629,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14"/>
@@ -1823,7 +1643,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>16837</v>
@@ -1838,7 +1658,7 @@
         <v>72</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15"/>
@@ -1852,7 +1672,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>17485</v>
@@ -1867,7 +1687,7 @@
         <v>248</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16"/>
@@ -1881,7 +1701,7 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>1430171</v>
@@ -1896,7 +1716,7 @@
         <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17"/>
@@ -1910,7 +1730,7 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>15288</v>
@@ -1925,7 +1745,7 @@
         <v>117</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18"/>
@@ -1939,7 +1759,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D19">
         <v>17558</v>
@@ -1954,7 +1774,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19"/>
@@ -1968,7 +1788,7 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="D20">
         <v>24988</v>
@@ -1983,7 +1803,7 @@
         <v>35</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20"/>
@@ -1997,7 +1817,7 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>878596</v>
@@ -2012,7 +1832,7 @@
         <v>567</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21"/>
@@ -2026,7 +1846,7 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D22">
         <v>15229</v>
@@ -2041,7 +1861,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22"/>
@@ -2055,7 +1875,7 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>15468</v>
@@ -2070,7 +1890,7 @@
         <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23"/>
@@ -2084,7 +1904,7 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="D24">
         <v>1356836</v>
@@ -2099,7 +1919,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24"/>
@@ -2113,7 +1933,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="D25">
         <v>1358987</v>
@@ -2128,7 +1948,7 @@
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25"/>
@@ -2142,7 +1962,7 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="D26">
         <v>22098</v>
@@ -2157,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="H26" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26"/>
@@ -2171,7 +1991,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="D27">
         <v>33065</v>
@@ -2186,7 +2006,7 @@
         <v>41</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27"/>
@@ -2200,7 +2020,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="D28">
         <v>34915</v>
@@ -2215,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28"/>
@@ -2229,7 +2049,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="D29">
         <v>1057456</v>
@@ -2244,7 +2064,7 @@
         <v>33</v>
       </c>
       <c r="H29" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2255,7 +2075,7 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>1122452</v>
@@ -2270,7 +2090,7 @@
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2281,7 +2101,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="D31">
         <v>11879</v>
@@ -2296,7 +2116,7 @@
         <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2307,7 +2127,7 @@
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="D32">
         <v>1055585</v>
@@ -2322,7 +2142,7 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2333,7 +2153,7 @@
         <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="D33">
         <v>34725</v>
@@ -2348,7 +2168,7 @@
         <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2359,7 +2179,7 @@
         <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>33729</v>
@@ -2374,7 +2194,7 @@
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2385,7 +2205,7 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="D35">
         <v>1122398</v>
@@ -2400,7 +2220,7 @@
         <v>17</v>
       </c>
       <c r="H35" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2411,7 +2231,7 @@
         <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="D36">
         <v>1057502</v>
@@ -2426,7 +2246,7 @@
         <v>23</v>
       </c>
       <c r="H36" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2437,7 +2257,7 @@
         <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="D37">
         <v>1373030</v>
@@ -2452,7 +2272,7 @@
         <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2463,7 +2283,7 @@
         <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="D38">
         <v>1261754</v>
@@ -2478,7 +2298,7 @@
         <v>16</v>
       </c>
       <c r="H38" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2489,7 +2309,7 @@
         <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="D39">
         <v>737267</v>
@@ -2504,7 +2324,7 @@
         <v>28</v>
       </c>
       <c r="H39" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2515,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D40">
         <v>737658</v>
@@ -2530,7 +2350,7 @@
         <v>23</v>
       </c>
       <c r="H40" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2541,7 +2361,7 @@
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="D41">
         <v>33521</v>
@@ -2556,7 +2376,7 @@
         <v>27</v>
       </c>
       <c r="H41" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2567,7 +2387,7 @@
         <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="D42">
         <v>34722</v>
@@ -2582,7 +2402,7 @@
         <v>137</v>
       </c>
       <c r="H42" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2593,7 +2413,7 @@
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="D43">
         <v>621498</v>
@@ -2619,7 +2439,7 @@
         <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="D44">
         <v>30321</v>
@@ -2671,7 +2491,7 @@
         <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="D46">
         <v>21986</v>
@@ -2697,7 +2517,7 @@
         <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="D47">
         <v>1145991</v>
@@ -2723,7 +2543,7 @@
         <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="D48">
         <v>14736</v>
@@ -2749,7 +2569,7 @@
         <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="D49">
         <v>622460</v>
@@ -2775,7 +2595,7 @@
         <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="D50">
         <v>24903</v>
@@ -2801,7 +2621,7 @@
         <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D51">
         <v>38069</v>
@@ -2827,7 +2647,7 @@
         <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="D52">
         <v>38070</v>
@@ -2853,7 +2673,7 @@
         <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="D53">
         <v>1429847</v>
@@ -2879,7 +2699,7 @@
         <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="D54">
         <v>22744</v>
@@ -2905,7 +2725,7 @@
         <v>27</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="D55">
         <v>623300</v>
@@ -2931,7 +2751,7 @@
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="D56">
         <v>623628</v>
@@ -2957,7 +2777,7 @@
         <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="D57">
         <v>985090</v>
@@ -2983,7 +2803,7 @@
         <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="D58">
         <v>16697</v>
@@ -3009,7 +2829,7 @@
         <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="D59">
         <v>1309013</v>
@@ -3035,7 +2855,7 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D60">
         <v>28968</v>
@@ -3061,7 +2881,7 @@
         <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D61">
         <v>33292</v>
@@ -3087,7 +2907,7 @@
         <v>27</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="D62">
         <v>26268</v>
@@ -3113,7 +2933,7 @@
         <v>27</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="D63">
         <v>678724</v>
@@ -3139,7 +2959,7 @@
         <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="D64">
         <v>1363719</v>
@@ -3165,7 +2985,7 @@
         <v>27</v>
       </c>
       <c r="C65" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="D65">
         <v>20860</v>
@@ -3191,7 +3011,7 @@
         <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="D66">
         <v>1303392</v>
@@ -3217,7 +3037,7 @@
         <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D67">
         <v>684449</v>
@@ -3243,7 +3063,7 @@
         <v>27</v>
       </c>
       <c r="C68" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="D68">
         <v>684759</v>
@@ -3269,7 +3089,7 @@
         <v>27</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="D69">
         <v>685011</v>
@@ -3295,7 +3115,7 @@
         <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
       <c r="D70">
         <v>1201239</v>
@@ -3321,7 +3141,7 @@
         <v>27</v>
       </c>
       <c r="C71" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="D71">
         <v>37709</v>
@@ -3347,7 +3167,7 @@
         <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="D72">
         <v>204374</v>
@@ -3373,7 +3193,7 @@
         <v>27</v>
       </c>
       <c r="C73" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
       <c r="D73">
         <v>1429784</v>
@@ -3399,7 +3219,7 @@
         <v>27</v>
       </c>
       <c r="C74" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="D74">
         <v>1126709</v>
@@ -3425,7 +3245,7 @@
         <v>27</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="D75">
         <v>875686</v>
@@ -3451,7 +3271,7 @@
         <v>27</v>
       </c>
       <c r="C76" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="D76">
         <v>1139037</v>
@@ -3477,7 +3297,7 @@
         <v>27</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="D77">
         <v>1139029</v>
@@ -3503,7 +3323,7 @@
         <v>27</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="D78">
         <v>1034235</v>
@@ -3529,7 +3349,7 @@
         <v>27</v>
       </c>
       <c r="C79" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="D79">
         <v>37906</v>
@@ -3555,7 +3375,7 @@
         <v>27</v>
       </c>
       <c r="C80" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="D80">
         <v>35519</v>
@@ -3581,7 +3401,7 @@
         <v>27</v>
       </c>
       <c r="C81" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D81">
         <v>679976</v>
@@ -3607,7 +3427,7 @@
         <v>27</v>
       </c>
       <c r="C82" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="D82">
         <v>1211935</v>
@@ -3633,7 +3453,7 @@
         <v>27</v>
       </c>
       <c r="C83" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="D83">
         <v>940607</v>
@@ -3659,7 +3479,7 @@
         <v>27</v>
       </c>
       <c r="C84" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="D84">
         <v>1352296</v>
@@ -3685,7 +3505,7 @@
         <v>27</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="D85">
         <v>12926</v>
@@ -3711,7 +3531,7 @@
         <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="D86">
         <v>690732</v>
@@ -3737,7 +3557,7 @@
         <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="D87">
         <v>37016</v>
@@ -3763,7 +3583,7 @@
         <v>27</v>
       </c>
       <c r="C88" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="D88">
         <v>686816</v>
@@ -3789,7 +3609,7 @@
         <v>27</v>
       </c>
       <c r="C89" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="D89">
         <v>1431996</v>
@@ -3815,7 +3635,7 @@
         <v>27</v>
       </c>
       <c r="C90" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="D90">
         <v>706876</v>
@@ -3841,7 +3661,7 @@
         <v>27</v>
       </c>
       <c r="C91" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="D91">
         <v>21745</v>
@@ -3867,7 +3687,7 @@
         <v>27</v>
       </c>
       <c r="C92" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="D92">
         <v>1218255</v>
@@ -3919,7 +3739,7 @@
         <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="D94">
         <v>31967</v>
@@ -3945,7 +3765,7 @@
         <v>27</v>
       </c>
       <c r="C95" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="D95">
         <v>36124</v>
@@ -4049,7 +3869,7 @@
         <v>27</v>
       </c>
       <c r="C99" t="s">
-        <v>184</v>
+        <v>124</v>
       </c>
       <c r="D99">
         <v>19673</v>
@@ -4075,7 +3895,7 @@
         <v>27</v>
       </c>
       <c r="C100" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="D100">
         <v>38156</v>
@@ -4101,7 +3921,7 @@
         <v>27</v>
       </c>
       <c r="C101" t="s">
-        <v>186</v>
+        <v>126</v>
       </c>
       <c r="D101">
         <v>38157</v>
@@ -4127,7 +3947,7 @@
         <v>27</v>
       </c>
       <c r="C102" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="D102">
         <v>26722</v>
@@ -4153,7 +3973,7 @@
         <v>27</v>
       </c>
       <c r="C103" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="D103">
         <v>1432597</v>
@@ -4179,7 +3999,7 @@
         <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="D104">
         <v>34572</v>
@@ -4205,7 +4025,7 @@
         <v>27</v>
       </c>
       <c r="C105" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="D105">
         <v>1250930</v>
@@ -4231,7 +4051,7 @@
         <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>191</v>
+        <v>131</v>
       </c>
       <c r="D106">
         <v>1250949</v>
@@ -4257,7 +4077,7 @@
         <v>27</v>
       </c>
       <c r="C107" t="s">
-        <v>192</v>
+        <v>132</v>
       </c>
       <c r="D107">
         <v>34718</v>
@@ -4283,7 +4103,7 @@
         <v>27</v>
       </c>
       <c r="C108" t="s">
-        <v>193</v>
+        <v>133</v>
       </c>
       <c r="D108">
         <v>735400</v>
@@ -4309,7 +4129,7 @@
         <v>27</v>
       </c>
       <c r="C109" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="D109">
         <v>1325329</v>
@@ -4335,7 +4155,7 @@
         <v>27</v>
       </c>
       <c r="C110" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D110">
         <v>1432312</v>
@@ -4361,7 +4181,7 @@
         <v>27</v>
       </c>
       <c r="C111" t="s">
-        <v>196</v>
+        <v>136</v>
       </c>
       <c r="D111">
         <v>30764</v>
@@ -4387,7 +4207,7 @@
         <v>27</v>
       </c>
       <c r="C112" t="s">
-        <v>197</v>
+        <v>137</v>
       </c>
       <c r="D112">
         <v>1222740</v>
@@ -4413,7 +4233,7 @@
         <v>27</v>
       </c>
       <c r="C113" t="s">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="D113">
         <v>37962</v>
@@ -4439,7 +4259,7 @@
         <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>199</v>
+        <v>139</v>
       </c>
       <c r="D114">
         <v>1129465</v>
@@ -4465,7 +4285,7 @@
         <v>27</v>
       </c>
       <c r="C115" t="s">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="D115">
         <v>1299000</v>
@@ -4491,7 +4311,7 @@
         <v>27</v>
       </c>
       <c r="C116" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="D116">
         <v>15234</v>
@@ -4517,7 +4337,7 @@
         <v>27</v>
       </c>
       <c r="C117" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="D117">
         <v>30692</v>
@@ -4543,7 +4363,7 @@
         <v>27</v>
       </c>
       <c r="C118" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="D118">
         <v>23128</v>
@@ -4569,7 +4389,7 @@
         <v>27</v>
       </c>
       <c r="C119" t="s">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="D119">
         <v>617784</v>
@@ -4595,7 +4415,7 @@
         <v>27</v>
       </c>
       <c r="C120" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="D120">
         <v>16841</v>
@@ -4621,7 +4441,7 @@
         <v>27</v>
       </c>
       <c r="C121" t="s">
-        <v>206</v>
+        <v>146</v>
       </c>
       <c r="D121">
         <v>19888</v>
@@ -4647,7 +4467,7 @@
         <v>27</v>
       </c>
       <c r="C122" t="s">
-        <v>207</v>
+        <v>147</v>
       </c>
       <c r="D122">
         <v>23029</v>
@@ -4673,7 +4493,7 @@
         <v>27</v>
       </c>
       <c r="C123" t="s">
-        <v>208</v>
+        <v>148</v>
       </c>
       <c r="D123">
         <v>23032</v>
@@ -4699,7 +4519,7 @@
         <v>27</v>
       </c>
       <c r="C124" t="s">
-        <v>209</v>
+        <v>149</v>
       </c>
       <c r="D124">
         <v>21423</v>
@@ -4725,7 +4545,7 @@
         <v>27</v>
       </c>
       <c r="C125" t="s">
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="D125">
         <v>31093</v>
@@ -4751,7 +4571,7 @@
         <v>27</v>
       </c>
       <c r="C126" t="s">
-        <v>211</v>
+        <v>151</v>
       </c>
       <c r="D126">
         <v>32765</v>
@@ -4777,7 +4597,7 @@
         <v>27</v>
       </c>
       <c r="C127" t="s">
-        <v>212</v>
+        <v>152</v>
       </c>
       <c r="D127">
         <v>1420720</v>
@@ -4829,7 +4649,7 @@
         <v>27</v>
       </c>
       <c r="C129" t="s">
-        <v>213</v>
+        <v>153</v>
       </c>
       <c r="D129">
         <v>33398</v>
@@ -4855,7 +4675,7 @@
         <v>27</v>
       </c>
       <c r="C130" t="s">
-        <v>214</v>
+        <v>154</v>
       </c>
       <c r="D130">
         <v>956678</v>
@@ -4881,7 +4701,7 @@
         <v>27</v>
       </c>
       <c r="C131" t="s">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="D131">
         <v>20697</v>
@@ -4907,7 +4727,7 @@
         <v>27</v>
       </c>
       <c r="C132" t="s">
-        <v>216</v>
+        <v>156</v>
       </c>
       <c r="D132">
         <v>724700</v>
@@ -4933,7 +4753,7 @@
         <v>27</v>
       </c>
       <c r="C133" t="s">
-        <v>217</v>
+        <v>157</v>
       </c>
       <c r="D133">
         <v>724602</v>
@@ -4959,7 +4779,7 @@
         <v>27</v>
       </c>
       <c r="C134" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
       <c r="D134">
         <v>725536</v>
@@ -4985,7 +4805,7 @@
         <v>27</v>
       </c>
       <c r="C135" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="D135">
         <v>1331523</v>
@@ -5011,7 +4831,7 @@
         <v>27</v>
       </c>
       <c r="C136" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
       <c r="D136">
         <v>31204</v>
@@ -5037,7 +4857,7 @@
         <v>27</v>
       </c>
       <c r="C137" t="s">
-        <v>221</v>
+        <v>161</v>
       </c>
       <c r="D137">
         <v>717207</v>
@@ -5063,7 +4883,7 @@
         <v>27</v>
       </c>
       <c r="C138" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="D138">
         <v>717231</v>
@@ -5089,7 +4909,7 @@
         <v>27</v>
       </c>
       <c r="C139" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
       <c r="D139">
         <v>33799</v>
@@ -5115,7 +4935,7 @@
         <v>27</v>
       </c>
       <c r="C140" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
       <c r="D140">
         <v>19443</v>
@@ -5141,7 +4961,7 @@
         <v>27</v>
       </c>
       <c r="C141" t="s">
-        <v>225</v>
+        <v>165</v>
       </c>
       <c r="D141">
         <v>1371380</v>
@@ -5167,7 +4987,7 @@
         <v>27</v>
       </c>
       <c r="C142" t="s">
-        <v>226</v>
+        <v>166</v>
       </c>
       <c r="D142">
         <v>1351729</v>
@@ -5193,7 +5013,7 @@
         <v>27</v>
       </c>
       <c r="C143" t="s">
-        <v>227</v>
+        <v>167</v>
       </c>
       <c r="D143">
         <v>1420879</v>
@@ -5219,7 +5039,7 @@
         <v>27</v>
       </c>
       <c r="C144" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="D144">
         <v>1428434</v>
@@ -5245,7 +5065,7 @@
         <v>27</v>
       </c>
       <c r="C145" t="s">
-        <v>229</v>
+        <v>169</v>
       </c>
       <c r="D145">
         <v>1205706</v>
@@ -5271,7 +5091,7 @@
         <v>27</v>
       </c>
       <c r="C146" t="s">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="D146">
         <v>35233</v>
@@ -5297,7 +5117,7 @@
         <v>27</v>
       </c>
       <c r="C147" t="s">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="D147">
         <v>848220</v>
@@ -5323,7 +5143,7 @@
         <v>27</v>
       </c>
       <c r="C148" t="s">
-        <v>232</v>
+        <v>172</v>
       </c>
       <c r="D148">
         <v>1402986</v>
@@ -5349,7 +5169,7 @@
         <v>27</v>
       </c>
       <c r="C149" t="s">
-        <v>233</v>
+        <v>173</v>
       </c>
       <c r="D149">
         <v>34898</v>
@@ -5375,7 +5195,7 @@
         <v>27</v>
       </c>
       <c r="C150" t="s">
-        <v>234</v>
+        <v>174</v>
       </c>
       <c r="D150">
         <v>36153</v>
@@ -5401,7 +5221,7 @@
         <v>27</v>
       </c>
       <c r="C151" t="s">
-        <v>235</v>
+        <v>175</v>
       </c>
       <c r="D151">
         <v>21212</v>
@@ -5427,7 +5247,7 @@
         <v>27</v>
       </c>
       <c r="C152" t="s">
-        <v>236</v>
+        <v>176</v>
       </c>
       <c r="D152">
         <v>27964</v>
@@ -5453,7 +5273,7 @@
         <v>27</v>
       </c>
       <c r="C153" t="s">
-        <v>237</v>
+        <v>177</v>
       </c>
       <c r="D153">
         <v>720585</v>
@@ -5479,7 +5299,7 @@
         <v>27</v>
       </c>
       <c r="C154" t="s">
-        <v>238</v>
+        <v>178</v>
       </c>
       <c r="D154">
         <v>37914</v>
@@ -5505,7 +5325,7 @@
         <v>27</v>
       </c>
       <c r="C155" t="s">
-        <v>239</v>
+        <v>179</v>
       </c>
       <c r="D155">
         <v>1060554</v>
@@ -5531,7 +5351,7 @@
         <v>27</v>
       </c>
       <c r="C156" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="D156">
         <v>33923</v>
@@ -5557,7 +5377,7 @@
         <v>27</v>
       </c>
       <c r="C157" t="s">
-        <v>241</v>
+        <v>181</v>
       </c>
       <c r="D157">
         <v>847402</v>
@@ -5609,7 +5429,7 @@
         <v>27</v>
       </c>
       <c r="C159" t="s">
-        <v>242</v>
+        <v>182</v>
       </c>
       <c r="D159">
         <v>697583</v>
@@ -5635,7 +5455,7 @@
         <v>27</v>
       </c>
       <c r="C160" t="s">
-        <v>243</v>
+        <v>183</v>
       </c>
       <c r="D160">
         <v>1029304</v>
@@ -5661,7 +5481,7 @@
         <v>27</v>
       </c>
       <c r="C161" t="s">
-        <v>244</v>
+        <v>184</v>
       </c>
       <c r="D161">
         <v>10580</v>
@@ -5687,7 +5507,7 @@
         <v>27</v>
       </c>
       <c r="C162" t="s">
-        <v>245</v>
+        <v>185</v>
       </c>
       <c r="D162">
         <v>1253808</v>
@@ -5713,7 +5533,7 @@
         <v>27</v>
       </c>
       <c r="C163" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="D163">
         <v>1253948</v>
@@ -5739,7 +5559,7 @@
         <v>27</v>
       </c>
       <c r="C164" t="s">
-        <v>247</v>
+        <v>187</v>
       </c>
       <c r="D164">
         <v>700673</v>
@@ -5765,7 +5585,7 @@
         <v>27</v>
       </c>
       <c r="C165" t="s">
-        <v>248</v>
+        <v>188</v>
       </c>
       <c r="D165">
         <v>1323989</v>
@@ -5780,7 +5600,7 @@
         <v>14</v>
       </c>
       <c r="H165" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
@@ -5791,7 +5611,7 @@
         <v>27</v>
       </c>
       <c r="C166" t="s">
-        <v>250</v>
+        <v>190</v>
       </c>
       <c r="D166">
         <v>14861</v>
@@ -5806,7 +5626,7 @@
         <v>27</v>
       </c>
       <c r="H166" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
@@ -5817,7 +5637,7 @@
         <v>27</v>
       </c>
       <c r="C167" t="s">
-        <v>251</v>
+        <v>191</v>
       </c>
       <c r="D167">
         <v>249289</v>
@@ -5832,18 +5652,18 @@
         <v>110</v>
       </c>
       <c r="H167" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B168" t="s">
         <v>27</v>
       </c>
       <c r="C168" t="s">
-        <v>252</v>
+        <v>192</v>
       </c>
       <c r="D168">
         <v>17736</v>
@@ -5858,18 +5678,18 @@
         <v>90</v>
       </c>
       <c r="H168" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B169" t="s">
         <v>27</v>
       </c>
       <c r="C169" t="s">
-        <v>253</v>
+        <v>193</v>
       </c>
       <c r="D169">
         <v>34037</v>
@@ -5884,18 +5704,18 @@
         <v>103</v>
       </c>
       <c r="H169" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B170" t="s">
         <v>27</v>
       </c>
       <c r="C170" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="D170">
         <v>15933</v>
@@ -5910,18 +5730,18 @@
         <v>14</v>
       </c>
       <c r="H170" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B171" t="s">
         <v>27</v>
       </c>
       <c r="C171" t="s">
-        <v>255</v>
+        <v>195</v>
       </c>
       <c r="D171">
         <v>37002</v>
@@ -5936,18 +5756,18 @@
         <v>25</v>
       </c>
       <c r="H171" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B172" t="s">
         <v>27</v>
       </c>
       <c r="C172" t="s">
-        <v>256</v>
+        <v>196</v>
       </c>
       <c r="D172">
         <v>35247</v>
@@ -5967,13 +5787,13 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B173" t="s">
         <v>27</v>
       </c>
       <c r="C173" t="s">
-        <v>257</v>
+        <v>197</v>
       </c>
       <c r="D173">
         <v>1154257</v>
@@ -5993,13 +5813,13 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B174" t="s">
         <v>27</v>
       </c>
       <c r="C174" t="s">
-        <v>258</v>
+        <v>198</v>
       </c>
       <c r="D174">
         <v>10808</v>
@@ -6019,7 +5839,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B175" t="s">
         <v>27</v>
@@ -6045,13 +5865,13 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B176" t="s">
         <v>27</v>
       </c>
       <c r="C176" t="s">
-        <v>259</v>
+        <v>199</v>
       </c>
       <c r="D176">
         <v>969494</v>
@@ -6071,13 +5891,13 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B177" t="s">
         <v>27</v>
       </c>
       <c r="C177" t="s">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D177">
         <v>1224204</v>
@@ -6097,13 +5917,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B178" t="s">
         <v>27</v>
       </c>
       <c r="C178" t="s">
-        <v>261</v>
+        <v>201</v>
       </c>
       <c r="D178">
         <v>643327</v>
@@ -6123,13 +5943,13 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B179" t="s">
         <v>27</v>
       </c>
       <c r="C179" t="s">
-        <v>262</v>
+        <v>202</v>
       </c>
       <c r="D179">
         <v>26168</v>
@@ -6149,13 +5969,13 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B180" t="s">
         <v>27</v>
       </c>
       <c r="C180" t="s">
-        <v>263</v>
+        <v>203</v>
       </c>
       <c r="D180">
         <v>1291718</v>
@@ -6175,13 +5995,13 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B181" t="s">
         <v>27</v>
       </c>
       <c r="C181" t="s">
-        <v>264</v>
+        <v>204</v>
       </c>
       <c r="D181">
         <v>31404</v>
@@ -6201,13 +6021,13 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B182" t="s">
         <v>27</v>
       </c>
       <c r="C182" t="s">
-        <v>265</v>
+        <v>205</v>
       </c>
       <c r="D182">
         <v>1031589</v>
@@ -6227,13 +6047,13 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B183" t="s">
         <v>27</v>
       </c>
       <c r="C183" t="s">
-        <v>266</v>
+        <v>206</v>
       </c>
       <c r="D183">
         <v>669636</v>
@@ -6253,13 +6073,13 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B184" t="s">
         <v>27</v>
       </c>
       <c r="C184" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
       <c r="D184">
         <v>20793</v>
@@ -6279,13 +6099,13 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B185" t="s">
         <v>27</v>
       </c>
       <c r="C185" t="s">
-        <v>268</v>
+        <v>208</v>
       </c>
       <c r="D185">
         <v>676292</v>
@@ -6305,13 +6125,13 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B186" t="s">
         <v>27</v>
       </c>
       <c r="C186" t="s">
-        <v>269</v>
+        <v>209</v>
       </c>
       <c r="D186">
         <v>38099</v>
@@ -6331,13 +6151,13 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B187" t="s">
         <v>27</v>
       </c>
       <c r="C187" t="s">
-        <v>270</v>
+        <v>210</v>
       </c>
       <c r="D187">
         <v>1186329</v>
@@ -6357,13 +6177,13 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B188" t="s">
         <v>27</v>
       </c>
       <c r="C188" t="s">
-        <v>271</v>
+        <v>211</v>
       </c>
       <c r="D188">
         <v>651664</v>
@@ -6383,7 +6203,7 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B189" t="s">
         <v>27</v>
@@ -6409,13 +6229,13 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B190" t="s">
         <v>27</v>
       </c>
       <c r="C190" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="D190">
         <v>38102</v>
@@ -6435,13 +6255,13 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B191" t="s">
         <v>27</v>
       </c>
       <c r="C191" t="s">
-        <v>273</v>
+        <v>213</v>
       </c>
       <c r="D191">
         <v>38103</v>
@@ -6461,13 +6281,13 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B192" t="s">
         <v>27</v>
       </c>
       <c r="C192" t="s">
-        <v>274</v>
+        <v>214</v>
       </c>
       <c r="D192">
         <v>1385046</v>
@@ -6487,13 +6307,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B193" t="s">
         <v>27</v>
       </c>
       <c r="C193" t="s">
-        <v>275</v>
+        <v>215</v>
       </c>
       <c r="D193">
         <v>1178180</v>
@@ -6513,13 +6333,13 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B194" t="s">
         <v>27</v>
       </c>
       <c r="C194" t="s">
-        <v>276</v>
+        <v>216</v>
       </c>
       <c r="D194">
         <v>26162</v>
@@ -6539,13 +6359,13 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B195" t="s">
         <v>27</v>
       </c>
       <c r="C195" t="s">
-        <v>277</v>
+        <v>217</v>
       </c>
       <c r="D195">
         <v>38108</v>
@@ -6565,13 +6385,13 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B196" t="s">
         <v>27</v>
       </c>
       <c r="C196" t="s">
-        <v>278</v>
+        <v>218</v>
       </c>
       <c r="D196">
         <v>13688</v>
@@ -6591,13 +6411,13 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B197" t="s">
         <v>27</v>
       </c>
       <c r="C197" t="s">
-        <v>279</v>
+        <v>219</v>
       </c>
       <c r="D197">
         <v>631574</v>
@@ -6617,13 +6437,13 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B198" t="s">
         <v>27</v>
       </c>
       <c r="C198" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="D198">
         <v>29085</v>
@@ -6643,13 +6463,13 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B199" t="s">
         <v>27</v>
       </c>
       <c r="C199" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="D199">
         <v>1042220</v>
@@ -6669,7 +6489,7 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B200" t="s">
         <v>27</v>
@@ -6695,13 +6515,13 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B201" t="s">
         <v>27</v>
       </c>
       <c r="C201" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="D201">
         <v>1337114</v>
@@ -6721,13 +6541,13 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B202" t="s">
         <v>27</v>
       </c>
       <c r="C202" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="D202">
         <v>1362119</v>
@@ -6747,13 +6567,13 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B203" t="s">
         <v>27</v>
       </c>
       <c r="C203" t="s">
-        <v>284</v>
+        <v>224</v>
       </c>
       <c r="D203">
         <v>25331</v>
@@ -6773,13 +6593,13 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B204" t="s">
         <v>27</v>
       </c>
       <c r="C204" t="s">
-        <v>285</v>
+        <v>225</v>
       </c>
       <c r="D204">
         <v>1389050</v>
@@ -6799,13 +6619,13 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B205" t="s">
         <v>27</v>
       </c>
       <c r="C205" t="s">
-        <v>286</v>
+        <v>226</v>
       </c>
       <c r="D205">
         <v>1430130</v>
@@ -6825,13 +6645,13 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B206" t="s">
         <v>27</v>
       </c>
       <c r="C206" t="s">
-        <v>287</v>
+        <v>227</v>
       </c>
       <c r="D206">
         <v>1430129</v>
@@ -6851,13 +6671,13 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="B207" t="s">
         <v>27</v>
       </c>
       <c r="C207" t="s">
-        <v>288</v>
+        <v>228</v>
       </c>
       <c r="D207">
         <v>631140</v>
@@ -6877,13 +6697,13 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B208" t="s">
         <v>27</v>
       </c>
       <c r="C208" t="s">
-        <v>289</v>
+        <v>229</v>
       </c>
       <c r="D208">
         <v>631205</v>
@@ -6903,13 +6723,13 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="B209" t="s">
         <v>27</v>
       </c>
       <c r="C209" t="s">
-        <v>290</v>
+        <v>230</v>
       </c>
       <c r="D209">
         <v>920835</v>
@@ -6929,13 +6749,13 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="B210" t="s">
         <v>27</v>
       </c>
       <c r="C210" t="s">
-        <v>291</v>
+        <v>231</v>
       </c>
       <c r="D210">
         <v>1388363</v>
@@ -6955,7 +6775,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B211" t="s">
         <v>27</v>
@@ -6981,13 +6801,13 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B212" t="s">
         <v>27</v>
       </c>
       <c r="C212" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="D212">
         <v>1201433</v>
@@ -7007,13 +6827,13 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="B213" t="s">
         <v>27</v>
       </c>
       <c r="C213" t="s">
-        <v>293</v>
+        <v>233</v>
       </c>
       <c r="D213">
         <v>1430395</v>
@@ -7033,13 +6853,13 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B214" t="s">
         <v>27</v>
       </c>
       <c r="C214" t="s">
-        <v>294</v>
+        <v>234</v>
       </c>
       <c r="D214">
         <v>23116</v>
@@ -7059,13 +6879,13 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B215" t="s">
         <v>27</v>
       </c>
       <c r="C215" t="s">
-        <v>295</v>
+        <v>235</v>
       </c>
       <c r="D215">
         <v>1201417</v>
@@ -7085,13 +6905,13 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B216" t="s">
         <v>27</v>
       </c>
       <c r="C216" t="s">
-        <v>296</v>
+        <v>236</v>
       </c>
       <c r="D216">
         <v>1201409</v>
@@ -7111,13 +6931,13 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B217" t="s">
         <v>27</v>
       </c>
       <c r="C217" t="s">
-        <v>297</v>
+        <v>237</v>
       </c>
       <c r="D217">
         <v>1201425</v>
@@ -7137,13 +6957,13 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B218" t="s">
         <v>27</v>
       </c>
       <c r="C218" t="s">
-        <v>298</v>
+        <v>238</v>
       </c>
       <c r="D218">
         <v>971529</v>
@@ -7163,13 +6983,13 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B219" t="s">
         <v>27</v>
       </c>
       <c r="C219" t="s">
-        <v>299</v>
+        <v>239</v>
       </c>
       <c r="D219">
         <v>828718</v>
@@ -7189,13 +7009,13 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B220" t="s">
         <v>27</v>
       </c>
       <c r="C220" t="s">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="D220">
         <v>27816</v>
@@ -7215,13 +7035,13 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="B221" t="s">
         <v>27</v>
       </c>
       <c r="C221" t="s">
-        <v>301</v>
+        <v>241</v>
       </c>
       <c r="D221">
         <v>830011</v>
@@ -7241,13 +7061,13 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B222" t="s">
         <v>27</v>
       </c>
       <c r="C222" t="s">
-        <v>302</v>
+        <v>242</v>
       </c>
       <c r="D222">
         <v>1199870</v>
@@ -7267,13 +7087,13 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="B223" t="s">
         <v>27</v>
       </c>
       <c r="C223" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
       <c r="D223">
         <v>830100</v>
@@ -7293,13 +7113,13 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B224" t="s">
         <v>27</v>
       </c>
       <c r="C224" t="s">
-        <v>304</v>
+        <v>244</v>
       </c>
       <c r="D224">
         <v>830062</v>
@@ -7319,13 +7139,13 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="B225" t="s">
         <v>27</v>
       </c>
       <c r="C225" t="s">
-        <v>305</v>
+        <v>245</v>
       </c>
       <c r="D225">
         <v>829862</v>
@@ -7345,13 +7165,13 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="B226" t="s">
         <v>27</v>
       </c>
       <c r="C226" t="s">
-        <v>306</v>
+        <v>246</v>
       </c>
       <c r="D226">
         <v>19129</v>
@@ -7371,13 +7191,13 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B227" t="s">
         <v>27</v>
       </c>
       <c r="C227" t="s">
-        <v>307</v>
+        <v>247</v>
       </c>
       <c r="D227">
         <v>38130</v>

</xml_diff>